<commit_message>
tratando match VA e VR e inserindo novas condições de match
</commit_message>
<xml_diff>
--- a/data/data_clean/vagas_gupy_clean.xlsx
+++ b/data/data_clean/vagas_gupy_clean.xlsx
@@ -700,7 +700,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Auxílio desenvolvimento', 'Auxílio home office', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Auxílio desenvolvimento', 'Day off aniversário', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R3" t="n">
@@ -795,7 +795,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Consignado', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Consignado', 'Day off aniversário', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R4" t="n">
@@ -890,7 +890,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Consignado', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Consignado', 'Day off aniversário', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R5" t="n">
@@ -1365,7 +1365,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Convênio com empresas parceiras', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Convênio com empresas parceiras', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R10" t="n">
@@ -1460,7 +1460,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R11" t="n">
@@ -1646,7 +1646,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio home office', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R13" t="n">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R14" t="n">
@@ -1836,7 +1836,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Cesta de natal', 'Ginástica laboral', 'Previdência privada', 'Programa de remuneração variável', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Cesta de natal', 'Day off aniversário', 'Ginástica laboral', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Programa de remuneração variável', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R15" t="n">
@@ -1931,7 +1931,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio home office', 'Day off aniversário', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R16" t="n">
@@ -2117,7 +2117,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Auxílio farmácia', 'Auxílio home office', 'Participação nos Lucros ou Resultados', 'Programa de treinamentos', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Auxílio farmácia', 'Participação nos Lucros ou Resultados', 'Programa de treinamentos', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R18" t="n">
@@ -2397,7 +2397,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio home office', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio home office', 'Day off aniversário', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R21" t="n">
@@ -2674,7 +2674,7 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Auxílio academia', 'Auxílio creche']</t>
+          <t>['Assistência médica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio creche']</t>
         </is>
       </c>
       <c r="R24" t="n">
@@ -2769,7 +2769,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio home office', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R25" t="n">
@@ -2959,7 +2959,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>['Auxílio academia', 'Ginástica laboral', 'Restaurante interno', 'Seguro de vida']</t>
+          <t>['Auxílio academia', 'Day off aniversário', 'Ginástica laboral', 'Restaurante interno', 'Seguro de vida']</t>
         </is>
       </c>
       <c r="R27" t="n">
@@ -3054,7 +3054,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Seguro de vida', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R28" t="n">
@@ -3244,7 +3244,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio desenvolvimento', 'Convênio com empresas parceiras', 'Previdência privada', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio desenvolvimento', 'Convênio com empresas parceiras', 'Day off aniversário', 'Previdência privada', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R30" t="n">
@@ -3339,7 +3339,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio desenvolvimento', 'Convênio com empresas parceiras', 'Previdência privada', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio desenvolvimento', 'Convênio com empresas parceiras', 'Day off aniversário', 'Previdência privada', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R31" t="n">
@@ -3711,7 +3711,7 @@
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Auxílio desenvolvimento']</t>
+          <t>['Assistência médica', 'Assistência psicológia', 'Auxílio desenvolvimento']</t>
         </is>
       </c>
       <c r="R35" t="n">
@@ -3806,7 +3806,7 @@
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio farmácia', 'Ginástica laboral', 'Massoterapia', 'Participação nos Lucros ou Resultados', 'Restaurante interno', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio creche', 'Auxílio farmácia', 'Day off aniversário', 'Ginástica laboral', 'Massoterapia', 'Participação nos Lucros ou Resultados', 'Restaurante interno', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R36" t="n">
@@ -3992,7 +3992,7 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Convênio com empresas parceiras', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Convênio com empresas parceiras', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R38" t="n">
@@ -4544,7 +4544,11 @@
           <t>Não informado</t>
         </is>
       </c>
-      <c r="Q44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>['Vale-refeição']</t>
+        </is>
+      </c>
       <c r="R44" t="n">
         <v>6667309</v>
       </c>
@@ -4827,7 +4831,7 @@
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R47" t="n">
@@ -4922,7 +4926,7 @@
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R48" t="n">
@@ -5017,7 +5021,7 @@
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>['Auxílio home office', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Auxílio home office', 'Day off aniversário', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R49" t="n">
@@ -5202,7 +5206,7 @@
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio home office', 'Programa de remuneração variável', 'Sala de Jogos', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Day off aniversário', 'Programa de remuneração variável', 'Sala de Jogos', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R51" t="n">
@@ -5573,7 +5577,7 @@
       </c>
       <c r="Q55" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Auxílio farmácia', 'Clube de vantagens', 'Horário flexível', 'Previdência privada', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Auxílio farmácia', 'Clube de vantagens', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R55" t="n">
@@ -5668,7 +5672,7 @@
       </c>
       <c r="Q56" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio farmácia', 'Auxílio home office', 'Convênio com empresas parceiras', 'Seguro de vida', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio farmácia', 'Auxílio home office', 'Convênio com empresas parceiras', 'Day off aniversário', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R56" t="n">
@@ -5763,7 +5767,7 @@
       </c>
       <c r="Q57" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio farmácia', 'Convênio com empresas parceiras', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio farmácia', 'Convênio com empresas parceiras', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R57" t="n">
@@ -5858,7 +5862,7 @@
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio estacionamento', 'Auxílio fretado', 'Restaurante interno', 'Seguro de vida', 'Vale-alimentação', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio estacionamento', 'Auxílio fretado', 'Participação nos Lucros ou Resultados', 'Restaurante interno', 'Seguro de vida', 'Vale-alimentação', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R58" t="n">
@@ -6044,7 +6048,7 @@
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Convênio com empresas parceiras', 'Vale-alimentação']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Convênio com empresas parceiras', 'Vale-alimentação']</t>
         </is>
       </c>
       <c r="R60" t="n">
@@ -6229,7 +6233,7 @@
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio home office', 'Horário flexível', 'Massoterapia', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Programa de treinamentos', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio creche', 'Horário flexível', 'Massoterapia', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Programa de treinamentos', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R62" t="n">
@@ -6415,7 +6419,7 @@
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio home office', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio home office', 'Day off aniversário', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R64" t="n">
@@ -6510,7 +6514,7 @@
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Convênio com empresas parceiras', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio creche', 'Convênio com empresas parceiras', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R65" t="n">
@@ -6604,7 +6608,7 @@
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Convênio com empresas parceiras', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio creche', 'Convênio com empresas parceiras', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R66" t="n">
@@ -6698,7 +6702,7 @@
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>['Convênio com empresas parceiras', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Convênio com empresas parceiras', 'Day off aniversário', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R67" t="n">
@@ -6793,7 +6797,7 @@
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Auxílio estacionamento', 'Auxílio home office', 'Consignado', 'Participação nos Lucros ou Resultados', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Auxílio estacionamento', 'Consignado', 'Day off aniversário', 'Participação nos Lucros ou Resultados', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R68" t="n">
@@ -6888,7 +6892,7 @@
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio farmácia', 'Convênio com empresas parceiras', 'Programa de treinamentos', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio farmácia', 'Convênio com empresas parceiras', 'Programa de treinamentos', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R69" t="n">
@@ -7168,7 +7172,7 @@
       </c>
       <c r="Q72" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Auxílio creche', 'Auxílio home office']</t>
+          <t>['Assistência médica', 'Auxílio creche', 'Auxílio home office', 'Day off aniversário', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R72" t="n">
@@ -7358,7 +7362,7 @@
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio home office', 'Convênio com empresas parceiras', 'Previdência privada']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio home office', 'Convênio com empresas parceiras', 'Day off aniversário', 'Previdência privada', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R74" t="n">
@@ -7544,7 +7548,7 @@
       </c>
       <c r="Q76" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Auxílio farmácia', 'Auxílio home office', 'Horário flexível', 'Programa de treinamentos', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Auxílio farmácia', 'Auxílio home office', 'Day off aniversário', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Programa de treinamentos', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R76" t="n">
@@ -7915,7 +7919,7 @@
       </c>
       <c r="Q80" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Previdência privada', 'Refeitório', 'Seguro de vida', 'Vale-alimentação', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio desenvolvimento', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Refeitório', 'Seguro de vida', 'Vale-alimentação', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R80" t="n">
@@ -8101,7 +8105,7 @@
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>['Convênio com empresas parceiras', 'Ginástica laboral', 'Vale-refeição']</t>
+          <t>['Assistência psicológia', 'Convênio com empresas parceiras', 'Day off aniversário', 'Ginástica laboral', 'Participação nos Lucros ou Resultados', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R82" t="n">
@@ -8378,7 +8382,7 @@
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Auxílio home office', 'Café da manhã', 'Massoterapia', 'Programa de treinamentos', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Café da manhã', 'Massoterapia', 'Programa de treinamentos', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R85" t="n">
@@ -8654,7 +8658,7 @@
       </c>
       <c r="Q88" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio estacionamento', 'Auxílio home office', 'Horário flexível', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio estacionamento', 'Day off aniversário', 'Horário flexível', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R88" t="n">
@@ -8749,7 +8753,7 @@
       </c>
       <c r="Q89" t="inlineStr">
         <is>
-          <t>['Assistência odontológica', 'Auxílio academia', 'Clube de vantagens', 'Convênio com empresas parceiras', 'Seguro de vida']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Clube de vantagens', 'Convênio com empresas parceiras', 'Participação nos Lucros ou Resultados', 'Seguro de vida']</t>
         </is>
       </c>
       <c r="R89" t="n">
@@ -8844,7 +8848,7 @@
       </c>
       <c r="Q90" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio farmácia', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio farmácia', 'Day off aniversário', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R90" t="n">
@@ -9211,7 +9215,7 @@
       </c>
       <c r="Q94" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Auxílio desenvolvimento', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Auxílio desenvolvimento', 'Day off aniversário', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R94" t="n">
@@ -9488,7 +9492,7 @@
       </c>
       <c r="Q97" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio desenvolvimento', 'Auxílio estacionamento', 'Clube de vantagens', 'Programa de remuneração variável', 'Restaurante interno', 'Seguro de vida', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio desenvolvimento', 'Auxílio estacionamento', 'Clube de vantagens', 'Day off aniversário', 'Programa de remuneração variável', 'Restaurante interno', 'Seguro de vida', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R97" t="n">
@@ -9673,7 +9677,7 @@
       </c>
       <c r="Q99" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio home office', 'Horário flexível', 'Massoterapia', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Programa de treinamentos', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio creche', 'Horário flexível', 'Massoterapia', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Programa de treinamentos', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R99" t="n">
@@ -10044,7 +10048,7 @@
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Auxílio farmácia', 'Programa de treinamentos', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Auxílio farmácia', 'Day off aniversário', 'Programa de treinamentos', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R103" t="n">
@@ -10234,7 +10238,7 @@
       </c>
       <c r="Q105" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio farmácia', 'Convênio com empresas parceiras', 'Desconto em produtos', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio farmácia', 'Convênio com empresas parceiras', 'Day off aniversário', 'Desconto em produtos', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R105" t="n">
@@ -10515,7 +10519,7 @@
       </c>
       <c r="Q108" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio estacionamento', 'Auxílio fretado', 'Restaurante interno', 'Seguro de vida', 'Vale-alimentação', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio estacionamento', 'Auxílio fretado', 'Participação nos Lucros ou Resultados', 'Restaurante interno', 'Seguro de vida', 'Vale-alimentação', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R108" t="n">
@@ -10705,7 +10709,7 @@
       </c>
       <c r="Q110" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Cesta de natal', 'Ginástica laboral', 'Previdência privada', 'Programa de remuneração variável', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Cesta de natal', 'Day off aniversário', 'Ginástica laboral', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Programa de remuneração variável', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R110" t="n">
@@ -10800,7 +10804,7 @@
       </c>
       <c r="Q111" t="inlineStr">
         <is>
-          <t>['Convênio com empresas parceiras', 'Ginástica laboral', 'Vale-refeição']</t>
+          <t>['Assistência psicológia', 'Convênio com empresas parceiras', 'Day off aniversário', 'Ginástica laboral', 'Participação nos Lucros ou Resultados', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R111" t="n">
@@ -10990,7 +10994,7 @@
       </c>
       <c r="Q113" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Auxílio home office', 'Cesta de natal']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Auxílio home office', 'Cesta de natal', 'Day off aniversário', 'Participação nos Lucros ou Resultados', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R113" t="n">
@@ -11085,7 +11089,7 @@
       </c>
       <c r="Q114" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio home office', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio home office', 'Day off aniversário', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R114" t="n">
@@ -11180,7 +11184,7 @@
       </c>
       <c r="Q115" t="inlineStr">
         <is>
-          <t>['Assistência odontológica', 'Auxílio creche', 'Auxílio home office', 'Convênio com empresas parceiras', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Auxílio home office', 'Convênio com empresas parceiras', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R115" t="n">
@@ -11460,7 +11464,7 @@
       </c>
       <c r="Q118" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Seguro de vida', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Seguro de vida', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R118" t="n">
@@ -11650,7 +11654,7 @@
       </c>
       <c r="Q120" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio farmácia', 'Auxílio fretado', 'Auxílio home office', 'Clube de vantagens', 'Refeitório', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio farmácia', 'Auxílio fretado', 'Clube de vantagens', 'Day off aniversário', 'Refeitório', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R120" t="n">
@@ -11840,7 +11844,7 @@
       </c>
       <c r="Q122" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio home office', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Seguro de vida', 'Vale-alimentação', 'Vale-cultura', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Seguro de vida', 'Vale-alimentação', 'Vale-cultura', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R122" t="n">
@@ -12125,7 +12129,7 @@
       </c>
       <c r="Q125" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Clube de vantagens', 'Convênio com empresas parceiras', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio creche', 'Clube de vantagens', 'Convênio com empresas parceiras', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R125" t="n">
@@ -12309,7 +12313,7 @@
       </c>
       <c r="Q127" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio home office', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio home office', 'Day off aniversário', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R127" t="n">
@@ -12404,7 +12408,7 @@
       </c>
       <c r="Q128" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Auxílio home office', 'Café da manhã', 'Massoterapia', 'Programa de treinamentos', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Café da manhã', 'Massoterapia', 'Programa de treinamentos', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R128" t="n">
@@ -12499,7 +12503,7 @@
       </c>
       <c r="Q129" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Convênio com empresas parceiras', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Convênio com empresas parceiras', 'Participação nos Lucros ou Resultados', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R129" t="n">
@@ -12784,7 +12788,7 @@
       </c>
       <c r="Q132" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Auxílio estacionamento', 'Auxílio farmácia', 'Ginástica laboral', 'Previdência privada', 'Programa de treinamentos', 'Refeitório', 'Sala de Jogos', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio creche', 'Auxílio estacionamento', 'Auxílio farmácia', 'Ginástica laboral', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Programa de treinamentos', 'Refeitório', 'Sala de Jogos', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R132" t="n">
@@ -13522,7 +13526,7 @@
       </c>
       <c r="Q140" t="inlineStr">
         <is>
-          <t>['Clube de vantagens', 'Vale-refeição']</t>
+          <t>['Auxílio academia', 'Clube de vantagens', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R140" t="n">
@@ -13617,7 +13621,7 @@
       </c>
       <c r="Q141" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Restaurante interno', 'Seguro de vida', 'Vale-alimentação']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Participação nos Lucros ou Resultados', 'Restaurante interno', 'Seguro de vida', 'Vale-alimentação']</t>
         </is>
       </c>
       <c r="R141" t="n">
@@ -13803,7 +13807,7 @@
       </c>
       <c r="Q143" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio home office', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R143" t="n">
@@ -13993,7 +13997,7 @@
       </c>
       <c r="Q145" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Participação nos Lucros ou Resultados', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R145" t="n">
@@ -14088,7 +14092,7 @@
       </c>
       <c r="Q146" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio farmácia', 'Previdência privada', 'Programa de remuneração variável', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio farmácia', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Programa de remuneração variável', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R146" t="n">
@@ -14277,7 +14281,7 @@
       </c>
       <c r="Q148" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio estacionamento', 'Café da manhã', 'Participação nos Lucros ou Resultados', 'Refeitório', 'Seguro de vida', 'Vale-alimentação']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio estacionamento', 'Café da manhã', 'Participação nos Lucros ou Resultados', 'Refeitório', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R148" t="n">
@@ -14744,7 +14748,7 @@
       </c>
       <c r="Q153" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Auxílio desenvolvimento']</t>
+          <t>['Assistência médica', 'Assistência psicológia', 'Auxílio desenvolvimento']</t>
         </is>
       </c>
       <c r="R153" t="n">
@@ -15120,7 +15124,7 @@
       </c>
       <c r="Q157" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Clube de vantagens', 'Convênio com empresas parceiras', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio creche', 'Clube de vantagens', 'Convênio com empresas parceiras', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R157" t="n">
@@ -15215,7 +15219,7 @@
       </c>
       <c r="Q158" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R158" t="n">
@@ -15310,7 +15314,7 @@
       </c>
       <c r="Q159" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio home office', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio home office', 'Day off aniversário', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R159" t="n">
@@ -15405,7 +15409,7 @@
       </c>
       <c r="Q160" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Auxílio academia', 'Programa de remuneração variável']</t>
+          <t>['Assistência médica', 'Assistência psicológia', 'Auxílio academia', 'Programa de remuneração variável']</t>
         </is>
       </c>
       <c r="R160" t="n">
@@ -15686,7 +15690,7 @@
       </c>
       <c r="Q163" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio home office', 'Consignado', 'Horário flexível', 'Restaurante interno']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio home office', 'Consignado', 'Day off aniversário', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Restaurante interno']</t>
         </is>
       </c>
       <c r="R163" t="n">
@@ -15781,7 +15785,7 @@
       </c>
       <c r="Q164" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Clube de vantagens', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Clube de vantagens', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R164" t="n">
@@ -15971,7 +15975,7 @@
       </c>
       <c r="Q166" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Auxílio creche', 'Auxílio desenvolvimento', 'Auxílio fretado', 'Auxílio home office', 'Cesta de natal', 'Convênio com empresas parceiras', 'Previdência privada', 'Restaurante interno', 'Seguro de vida', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Auxílio creche', 'Auxílio desenvolvimento', 'Auxílio fretado', 'Cesta de natal', 'Convênio com empresas parceiras', 'Previdência privada', 'Restaurante interno', 'Seguro de vida', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R166" t="n">
@@ -16066,7 +16070,7 @@
       </c>
       <c r="Q167" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Auxílio home office', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Auxílio home office', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R167" t="n">
@@ -16161,7 +16165,7 @@
       </c>
       <c r="Q168" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Auxílio home office', 'Clube de vantagens', 'Convênio com empresas parceiras', 'Programa de remuneração variável', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Clube de vantagens', 'Convênio com empresas parceiras', 'Day off aniversário', 'Programa de remuneração variável', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R168" t="n">
@@ -16442,7 +16446,7 @@
       </c>
       <c r="Q171" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Clube de vantagens', 'Convênio com empresas parceiras', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio creche', 'Clube de vantagens', 'Convênio com empresas parceiras', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R171" t="n">
@@ -16537,7 +16541,7 @@
       </c>
       <c r="Q172" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Convênio com empresas parceiras', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio creche', 'Convênio com empresas parceiras', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R172" t="n">
@@ -16632,7 +16636,7 @@
       </c>
       <c r="Q173" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Day off aniversário', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R173" t="n">
@@ -16727,7 +16731,7 @@
       </c>
       <c r="Q174" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio home office', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio home office', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R174" t="n">
@@ -16822,7 +16826,7 @@
       </c>
       <c r="Q175" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio desenvolvimento', 'Horário flexível', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio desenvolvimento', 'Day off aniversário', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R175" t="n">
@@ -16917,7 +16921,7 @@
       </c>
       <c r="Q176" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio estacionamento', 'Auxílio fretado', 'Cesta básica', 'Restaurante interno', 'Seguro de vida', 'Vale-alimentação', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio estacionamento', 'Auxílio fretado', 'Cesta básica', 'Participação nos Lucros ou Resultados', 'Restaurante interno', 'Seguro de vida', 'Vale-alimentação', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R176" t="n">
@@ -17012,7 +17016,7 @@
       </c>
       <c r="Q177" t="inlineStr">
         <is>
-          <t>['Assistência odontológica', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Day off aniversário', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R177" t="n">
@@ -17107,7 +17111,7 @@
       </c>
       <c r="Q178" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Auxílio academia', 'Auxílio home office', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência psicológia', 'Auxílio academia', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R178" t="n">
@@ -17650,7 +17654,7 @@
       </c>
       <c r="Q184" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Consignado', 'Seguro de vida', 'Vale-alimentação']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Consignado', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação']</t>
         </is>
       </c>
       <c r="R184" t="n">
@@ -17745,7 +17749,7 @@
       </c>
       <c r="Q185" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Consignado', 'Seguro de vida', 'Vale-alimentação']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Consignado', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação']</t>
         </is>
       </c>
       <c r="R185" t="n">
@@ -17935,7 +17939,7 @@
       </c>
       <c r="Q187" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Auxílio farmácia', 'Seguro de vida', 'Vale-alimentação', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Auxílio farmácia', 'Seguro de vida', 'Vale-alimentação', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R187" t="n">
@@ -18030,7 +18034,7 @@
       </c>
       <c r="Q188" t="inlineStr">
         <is>
-          <t>['Assistência médica']</t>
+          <t>['Assistência médica', 'Day off aniversário', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R188" t="n">
@@ -18125,7 +18129,7 @@
       </c>
       <c r="Q189" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Auxílio academia', 'Auxílio home office', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Auxílio academia', 'Auxílio home office', 'Participação nos Lucros ou Resultados', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R189" t="n">
@@ -18313,11 +18317,7 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="Q191" t="inlineStr">
-        <is>
-          <t>['Auxílio home office']</t>
-        </is>
-      </c>
+      <c r="Q191" t="inlineStr"/>
       <c r="R191" t="n">
         <v>5195236</v>
       </c>
@@ -18596,7 +18596,7 @@
       </c>
       <c r="Q194" t="inlineStr">
         <is>
-          <t>['Assistência odontológica', 'Convênio com empresas parceiras', 'Seguro de vida']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Convênio com empresas parceiras', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R194" t="n">
@@ -18691,7 +18691,7 @@
       </c>
       <c r="Q195" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Clube de vantagens', 'Convênio com empresas parceiras', 'Programa de remuneração variável', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Clube de vantagens', 'Convênio com empresas parceiras', 'Day off aniversário', 'Programa de remuneração variável', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R195" t="n">
@@ -18786,7 +18786,7 @@
       </c>
       <c r="Q196" t="inlineStr">
         <is>
-          <t>['Auxílio desenvolvimento']</t>
+          <t>['Auxílio desenvolvimento', 'Day off aniversário']</t>
         </is>
       </c>
       <c r="R196" t="n">
@@ -19249,7 +19249,7 @@
       </c>
       <c r="Q201" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Horário flexível', 'Previdência privada', 'Programa de treinamentos', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio creche', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Programa de treinamentos', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R201" t="n">
@@ -19530,7 +19530,7 @@
       </c>
       <c r="Q204" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Auxílio academia', 'Auxílio home office', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência psicológia', 'Auxílio academia', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R204" t="n">
@@ -19789,7 +19789,7 @@
       </c>
       <c r="Q207" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Consignado', 'Cooperativa de crédito', 'Previdência privada', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Consignado', 'Cooperativa de crédito', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R207" t="n">
@@ -20219,7 +20219,7 @@
       </c>
       <c r="Q212" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio desenvolvimento', 'Horário flexível', 'Programa de treinamentos', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio desenvolvimento', 'Horário flexível', 'Programa de treinamentos', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R212" t="n">
@@ -20559,7 +20559,7 @@
       </c>
       <c r="Q216" t="inlineStr">
         <is>
-          <t>['Assistência odontológica', 'Auxílio academia', 'Auxílio desenvolvimento', 'Convênio com empresas parceiras', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Programa de treinamentos', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio desenvolvimento', 'Convênio com empresas parceiras', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Programa de treinamentos', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R216" t="n">
@@ -20654,7 +20654,7 @@
       </c>
       <c r="Q217" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio farmácia', 'Clube de vantagens', 'Consignado', 'Convênio com empresas parceiras', 'Ginástica laboral', 'Previdência privada', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio farmácia', 'Clube de vantagens', 'Consignado', 'Convênio com empresas parceiras', 'Day off aniversário', 'Ginástica laboral', 'Previdência privada', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R217" t="n">
@@ -20844,7 +20844,7 @@
       </c>
       <c r="Q219" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Participação nos Lucros ou Resultados', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio home office', 'Day off aniversário', 'Participação nos Lucros ou Resultados', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R219" t="n">
@@ -21034,7 +21034,7 @@
       </c>
       <c r="Q221" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Participação nos Lucros ou Resultados', 'Vale-alimentação']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Day off aniversário', 'Participação nos Lucros ou Resultados', 'Vale-alimentação']</t>
         </is>
       </c>
       <c r="R221" t="n">
@@ -21315,7 +21315,7 @@
       </c>
       <c r="Q224" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Café da manhã', 'Convênio com empresas parceiras', 'Ginástica laboral', 'Participação nos Lucros ou Resultados', 'Sala de Jogos']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Café da manhã', 'Convênio com empresas parceiras', 'Day off aniversário', 'Ginástica laboral', 'Participação nos Lucros ou Resultados', 'Sala de Jogos']</t>
         </is>
       </c>
       <c r="R224" t="n">
@@ -21500,7 +21500,7 @@
       </c>
       <c r="Q226" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Convênio com empresas parceiras', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Convênio com empresas parceiras', 'Day off aniversário', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R226" t="n">
@@ -21780,7 +21780,7 @@
       </c>
       <c r="Q229" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio home office', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio home office', 'Day off aniversário', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R229" t="n">
@@ -21965,7 +21965,7 @@
       </c>
       <c r="Q231" t="inlineStr">
         <is>
-          <t>['Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Auxílio academia', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R231" t="n">
@@ -22155,7 +22155,7 @@
       </c>
       <c r="Q233" t="inlineStr">
         <is>
-          <t>['Assistência odontológica', 'Auxílio academia', 'Auxílio desenvolvimento', 'Convênio com empresas parceiras', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Programa de treinamentos', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio desenvolvimento', 'Convênio com empresas parceiras', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Programa de treinamentos', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R233" t="n">
@@ -22250,7 +22250,7 @@
       </c>
       <c r="Q234" t="inlineStr">
         <is>
-          <t>['Assistência odontológica', 'Auxílio academia', 'Auxílio desenvolvimento', 'Convênio com empresas parceiras', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Programa de treinamentos', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio desenvolvimento', 'Convênio com empresas parceiras', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Programa de treinamentos', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R234" t="n">
@@ -22440,7 +22440,7 @@
       </c>
       <c r="Q236" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio estacionamento', 'Horário flexível', 'Restaurante interno', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio estacionamento', 'Day off aniversário', 'Horário flexível', 'Restaurante interno', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R236" t="n">
@@ -22626,7 +22626,7 @@
       </c>
       <c r="Q238" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Convênio com empresas parceiras', 'Vale-alimentação']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Convênio com empresas parceiras', 'Vale-alimentação']</t>
         </is>
       </c>
       <c r="R238" t="n">
@@ -22812,7 +22812,7 @@
       </c>
       <c r="Q240" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Auxílio academia', 'Auxílio home office', 'Convênio com empresas parceiras', 'Horário flexível']</t>
+          <t>['Assistência médica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio home office', 'Convênio com empresas parceiras', 'Day off aniversário', 'Horário flexível', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R240" t="n">
@@ -22907,7 +22907,7 @@
       </c>
       <c r="Q241" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Desconto em produtos', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Day off aniversário', 'Desconto em produtos', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R241" t="n">
@@ -23279,7 +23279,7 @@
       </c>
       <c r="Q245" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Ginástica laboral', 'Horário flexível', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio creche', 'Auxílio home office', 'Day off aniversário', 'Ginástica laboral', 'Horário flexível', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R245" t="n">
@@ -23374,7 +23374,7 @@
       </c>
       <c r="Q246" t="inlineStr">
         <is>
-          <t>['Assistência odontológica', 'Auxílio home office', 'Convênio com empresas parceiras', 'Previdência privada', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio home office', 'Convênio com empresas parceiras', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R246" t="n">
@@ -23469,7 +23469,7 @@
       </c>
       <c r="Q247" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Auxílio academia', 'Auxílio desenvolvimento', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio desenvolvimento', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R247" t="n">
@@ -23564,7 +23564,7 @@
       </c>
       <c r="Q248" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio farmácia', 'Auxílio home office', 'Horário flexível', 'Programa de treinamentos']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio farmácia', 'Auxílio home office', 'Horário flexível', 'Programa de treinamentos', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R248" t="n">
@@ -24212,7 +24212,7 @@
       </c>
       <c r="Q255" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Convênio com empresas parceiras', 'Seguro de vida', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Convênio com empresas parceiras', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R255" t="n">
@@ -24588,7 +24588,7 @@
       </c>
       <c r="Q259" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Auxílio academia', 'Auxílio creche', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Auxílio academia', 'Auxílio creche', 'Day off aniversário', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R259" t="n">
@@ -25136,7 +25136,7 @@
       </c>
       <c r="Q265" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Auxílio academia', 'Auxílio home office', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência psicológia', 'Auxílio academia', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R265" t="n">
@@ -25231,7 +25231,7 @@
       </c>
       <c r="Q266" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Consignado', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Consignado', 'Day off aniversário', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R266" t="n">
@@ -25326,7 +25326,7 @@
       </c>
       <c r="Q267" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Seguro de vida', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Seguro de vida', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R267" t="n">
@@ -25511,7 +25511,7 @@
       </c>
       <c r="Q269" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio farmácia', 'Auxílio fretado', 'Auxílio home office', 'Clube de vantagens', 'Refeitório', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio farmácia', 'Auxílio fretado', 'Clube de vantagens', 'Day off aniversário', 'Refeitório', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R269" t="n">
@@ -25978,7 +25978,7 @@
       </c>
       <c r="Q274" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Convênio com empresas parceiras', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Convênio com empresas parceiras', 'Participação nos Lucros ou Resultados', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R274" t="n">
@@ -26164,7 +26164,7 @@
       </c>
       <c r="Q276" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Auxílio academia', 'Auxílio home office', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência psicológia', 'Auxílio academia', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R276" t="n">
@@ -26259,7 +26259,7 @@
       </c>
       <c r="Q277" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Auxílio home office', 'Horário flexível', 'Vale-alimentação']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Horário flexível', 'Vale-alimentação']</t>
         </is>
       </c>
       <c r="R277" t="n">
@@ -26354,7 +26354,7 @@
       </c>
       <c r="Q278" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R278" t="n">
@@ -26449,7 +26449,7 @@
       </c>
       <c r="Q279" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Auxílio desenvolvimento', 'Auxílio home office', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Auxílio desenvolvimento', 'Day off aniversário', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R279" t="n">
@@ -26820,7 +26820,7 @@
       </c>
       <c r="Q283" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Auxílio estacionamento', 'Auxílio home office', 'Horário flexível', 'Programa de treinamentos', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Auxílio estacionamento', 'Auxílio home office', 'Day off aniversário', 'Horário flexível', 'Programa de treinamentos', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R283" t="n">
@@ -27006,7 +27006,7 @@
       </c>
       <c r="Q285" t="inlineStr">
         <is>
-          <t>['Assistência odontológica', 'Auxílio academia', 'Auxílio desenvolvimento', 'Convênio com empresas parceiras', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Programa de treinamentos', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio desenvolvimento', 'Convênio com empresas parceiras', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Programa de treinamentos', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R285" t="n">
@@ -27196,7 +27196,7 @@
       </c>
       <c r="Q287" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Auxílio desenvolvimento', 'Auxílio farmácia', 'Convênio com empresas parceiras', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Auxílio farmácia', 'Convênio com empresas parceiras', 'Day off aniversário', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R287" t="n">
@@ -27379,7 +27379,7 @@
       </c>
       <c r="Q289" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Auxílio estacionamento', 'Auxílio farmácia', 'Clube de vantagens', 'Horário flexível', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Auxílio desenvolvimento', 'Auxílio estacionamento', 'Auxílio farmácia', 'Clube de vantagens', 'Day off aniversário', 'Horário flexível', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R289" t="n">
@@ -27474,7 +27474,7 @@
       </c>
       <c r="Q290" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R290" t="n">
@@ -27659,7 +27659,7 @@
       </c>
       <c r="Q292" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Clube de vantagens', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Clube de vantagens', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R292" t="n">
@@ -28121,7 +28121,7 @@
       </c>
       <c r="Q297" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Auxílio home office', 'Horário flexível', 'Vale-alimentação']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Horário flexível', 'Vale-alimentação']</t>
         </is>
       </c>
       <c r="R297" t="n">
@@ -28216,7 +28216,7 @@
       </c>
       <c r="Q298" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Auxílio home office', 'Horário flexível', 'Vale-alimentação']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio desenvolvimento', 'Horário flexível', 'Vale-alimentação']</t>
         </is>
       </c>
       <c r="R298" t="n">
@@ -28402,7 +28402,7 @@
       </c>
       <c r="Q300" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio home office', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio home office', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R300" t="n">
@@ -28497,7 +28497,7 @@
       </c>
       <c r="Q301" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio creche', 'Clube de vantagens', 'Convênio com empresas parceiras', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio creche', 'Clube de vantagens', 'Convênio com empresas parceiras', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R301" t="n">
@@ -29134,7 +29134,7 @@
       </c>
       <c r="Q308" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Auxílio academia', 'Auxílio home office', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
+          <t>['Assistência médica', 'Assistência psicológia', 'Auxílio academia', 'Horário flexível', 'Participação nos Lucros ou Resultados', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição']</t>
         </is>
       </c>
       <c r="R308" t="n">
@@ -29663,7 +29663,7 @@
       </c>
       <c r="Q314" t="inlineStr">
         <is>
-          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio academia', 'Auxílio desenvolvimento', 'Horário flexível', 'Programa de treinamentos', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Assistência psicológia', 'Auxílio academia', 'Auxílio desenvolvimento', 'Horário flexível', 'Programa de treinamentos', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R314" t="n">

</xml_diff>

<commit_message>
tratando dados faltantes na coluna estado
</commit_message>
<xml_diff>
--- a/data/data_clean/vagas_gupy_clean.xlsx
+++ b/data/data_clean/vagas_gupy_clean.xlsx
@@ -864,7 +864,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -1054,7 +1054,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -2000,7 +2000,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -2091,7 +2091,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -2371,7 +2371,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -2557,7 +2557,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -2648,7 +2648,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -4520,7 +4520,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -4615,7 +4615,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -6207,7 +6207,7 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L62" t="inlineStr">
@@ -6302,7 +6302,7 @@
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L63" t="inlineStr">
@@ -7051,7 +7051,7 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
@@ -7146,7 +7146,7 @@
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L72" t="inlineStr">
@@ -7336,7 +7336,7 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
@@ -7522,7 +7522,7 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
@@ -8174,7 +8174,7 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
@@ -8727,7 +8727,7 @@
       </c>
       <c r="K89" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L89" t="inlineStr">
@@ -9651,7 +9651,7 @@
       </c>
       <c r="K99" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L99" t="inlineStr">
@@ -10588,7 +10588,7 @@
       </c>
       <c r="K109" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L109" t="inlineStr">
@@ -11063,7 +11063,7 @@
       </c>
       <c r="K114" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L114" t="inlineStr">
@@ -11253,7 +11253,7 @@
       </c>
       <c r="K116" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L116" t="inlineStr">
@@ -12103,7 +12103,7 @@
       </c>
       <c r="K125" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L125" t="inlineStr">
@@ -14817,7 +14817,7 @@
       </c>
       <c r="K154" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L154" t="inlineStr">
@@ -15383,7 +15383,7 @@
       </c>
       <c r="K160" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L160" t="inlineStr">
@@ -15664,7 +15664,7 @@
       </c>
       <c r="K163" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L163" t="inlineStr">
@@ -16139,7 +16139,7 @@
       </c>
       <c r="K168" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L168" t="inlineStr">
@@ -16420,7 +16420,7 @@
       </c>
       <c r="K171" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L171" t="inlineStr">
@@ -16705,7 +16705,7 @@
       </c>
       <c r="K174" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L174" t="inlineStr">
@@ -16800,7 +16800,7 @@
       </c>
       <c r="K175" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L175" t="inlineStr">
@@ -18103,7 +18103,7 @@
       </c>
       <c r="K189" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L189" t="inlineStr">
@@ -20723,7 +20723,7 @@
       </c>
       <c r="K218" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L218" t="inlineStr">
@@ -20818,7 +20818,7 @@
       </c>
       <c r="K219" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L219" t="inlineStr">
@@ -20913,7 +20913,7 @@
       </c>
       <c r="K220" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L220" t="inlineStr">
@@ -21103,7 +21103,7 @@
       </c>
       <c r="K222" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L222" t="inlineStr">
@@ -21198,7 +21198,7 @@
       </c>
       <c r="K223" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L223" t="inlineStr">
@@ -21384,7 +21384,7 @@
       </c>
       <c r="K225" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L225" t="inlineStr">
@@ -21474,7 +21474,7 @@
       </c>
       <c r="K226" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L226" t="inlineStr">
@@ -21569,7 +21569,7 @@
       </c>
       <c r="K227" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L227" t="inlineStr">
@@ -21754,7 +21754,7 @@
       </c>
       <c r="K229" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L229" t="inlineStr">
@@ -21849,7 +21849,7 @@
       </c>
       <c r="K230" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L230" t="inlineStr">
@@ -21939,7 +21939,7 @@
       </c>
       <c r="K231" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L231" t="inlineStr">
@@ -22414,7 +22414,7 @@
       </c>
       <c r="K236" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L236" t="inlineStr">
@@ -22509,7 +22509,7 @@
       </c>
       <c r="K237" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L237" t="inlineStr">
@@ -22695,7 +22695,7 @@
       </c>
       <c r="K239" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L239" t="inlineStr">
@@ -22786,7 +22786,7 @@
       </c>
       <c r="K240" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L240" t="inlineStr">
@@ -22976,7 +22976,7 @@
       </c>
       <c r="K242" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L242" t="inlineStr">
@@ -23067,7 +23067,7 @@
       </c>
       <c r="K243" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L243" t="inlineStr">
@@ -23158,7 +23158,7 @@
       </c>
       <c r="K244" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L244" t="inlineStr">
@@ -23253,7 +23253,7 @@
       </c>
       <c r="K245" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L245" t="inlineStr">
@@ -23443,7 +23443,7 @@
       </c>
       <c r="K247" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L247" t="inlineStr">
@@ -23538,7 +23538,7 @@
       </c>
       <c r="K248" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L248" t="inlineStr">
@@ -23633,7 +23633,7 @@
       </c>
       <c r="K249" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L249" t="inlineStr">
@@ -23728,7 +23728,7 @@
       </c>
       <c r="K250" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L250" t="inlineStr">
@@ -23910,7 +23910,7 @@
       </c>
       <c r="K252" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L252" t="inlineStr">
@@ -24657,7 +24657,7 @@
       </c>
       <c r="K260" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L260" t="inlineStr">
@@ -24839,7 +24839,7 @@
       </c>
       <c r="K262" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L262" t="inlineStr">
@@ -25110,7 +25110,7 @@
       </c>
       <c r="K265" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L265" t="inlineStr">
@@ -25395,7 +25395,7 @@
       </c>
       <c r="K268" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L268" t="inlineStr">
@@ -25766,7 +25766,7 @@
       </c>
       <c r="K272" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L272" t="inlineStr">
@@ -25861,7 +25861,7 @@
       </c>
       <c r="K273" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L273" t="inlineStr">
@@ -26047,7 +26047,7 @@
       </c>
       <c r="K275" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L275" t="inlineStr">
@@ -26138,7 +26138,7 @@
       </c>
       <c r="K276" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L276" t="inlineStr">
@@ -26233,7 +26233,7 @@
       </c>
       <c r="K277" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L277" t="inlineStr">
@@ -26423,7 +26423,7 @@
       </c>
       <c r="K279" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L279" t="inlineStr">
@@ -26518,7 +26518,7 @@
       </c>
       <c r="K280" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L280" t="inlineStr">
@@ -26889,7 +26889,7 @@
       </c>
       <c r="K284" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L284" t="inlineStr">
@@ -27265,7 +27265,7 @@
       </c>
       <c r="K288" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L288" t="inlineStr">
@@ -27353,7 +27353,7 @@
       </c>
       <c r="K289" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L289" t="inlineStr">
@@ -27543,7 +27543,7 @@
       </c>
       <c r="K291" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L291" t="inlineStr">
@@ -27728,7 +27728,7 @@
       </c>
       <c r="K293" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L293" t="inlineStr">
@@ -28095,7 +28095,7 @@
       </c>
       <c r="K297" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L297" t="inlineStr">
@@ -28190,7 +28190,7 @@
       </c>
       <c r="K298" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L298" t="inlineStr">
@@ -28376,7 +28376,7 @@
       </c>
       <c r="K300" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L300" t="inlineStr">
@@ -28471,7 +28471,7 @@
       </c>
       <c r="K301" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L301" t="inlineStr">
@@ -29637,7 +29637,7 @@
       </c>
       <c r="K314" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Todo o Brasil</t>
         </is>
       </c>
       <c r="L314" t="inlineStr">

</xml_diff>